<commit_message>
Habilitando CORS en la API
</commit_message>
<xml_diff>
--- a/generated_report.xlsx
+++ b/generated_report.xlsx
@@ -180,12 +180,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Reporte'!$A$2:$A$5</f>
+              <f>'Reporte'!$A$2</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Reporte'!$B$2:$B$5</f>
+              <f>'Reporte'!$B$2</f>
             </numRef>
           </val>
         </ser>
@@ -541,7 +541,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -551,63 +551,44 @@
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Categoría</t>
+          <t>nombre</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Ingresos</t>
+          <t>edad</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ciudad</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ventas</t>
+          <t>Erick</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>50000</v>
+        <v>28</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Mérida</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Marketing</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Operaciones</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Finanzas</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="2">
-        <f>SUM(B2:B5)</f>
+      <c r="B3" s="2">
+        <f>SUM(B2:B2)</f>
         <v/>
       </c>
     </row>

</xml_diff>